<commit_message>
Alter bei AN-Anteil PV hinzugefügt und notwendige Änderungen vorgenommen. Alle Tests laufen
</commit_message>
<xml_diff>
--- a/src/main/2 insert Sozialversicherungsdaten/5 Anzahl Kinder Arbeitnehmer PV-Beitrag.xlsx
+++ b/src/main/2 insert Sozialversicherungsdaten/5 Anzahl Kinder Arbeitnehmer PV-Beitrag.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\2 insert Sozialversicherungsdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B81D70C-2A14-4625-80BF-70ACBC8B1120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFCF9D5-A507-47F3-BFCA-ADAA578447B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35850" yWindow="3300" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Daten</t>
   </si>
@@ -49,6 +50,18 @@
   </si>
   <si>
     <t>01.01.2024</t>
+  </si>
+  <si>
+    <t>Juenger als 23 oder geboren vor 1940</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>nein</t>
   </si>
 </sst>
 </file>
@@ -378,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,38 +421,88 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1.7</v>
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>62100</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>69300</v>
+        <v>62100</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>69300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{82B51A73-C65F-49EE-9FF2-9C2CEEB47183}">
+          <x14:formula1>
+            <xm:f>Tabelle2!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{705EB0E1-478D-423B-B721-C4722C4AE4FC}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>